<commit_message>
add new result leson and debug solved [not sorted]
</commit_message>
<xml_diff>
--- a/quiz.xlsx
+++ b/quiz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Persons\Soroosh\Quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4859F7-3FEE-4A79-B583-A9172FA23DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654D88EA-63E6-44DB-BA6E-1C0E4155FBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -986,17 +986,17 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill>
@@ -1099,27 +1099,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3955,7 +3934,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5376,7 +5355,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5588,21 +5567,21 @@
         <v>69</v>
       </c>
       <c r="B7" s="21">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="45" t="s">
         <v>203</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
@@ -6059,7 +6038,7 @@
   <dimension ref="A1:BK26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12630,7 +12609,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12714,7 +12693,7 @@
       </c>
       <c r="H5" s="7">
         <f>INDEX('کارنامه فردی'!L2:L26,MATCH('نتیجه فردی'!$B$1,'کارنامه فردی'!$A$2:$A$26,0))</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -12748,7 +12727,7 @@
       </c>
       <c r="H6" s="7">
         <f>INDEX('کارنامه فردی'!U2:U26,MATCH('نتیجه فردی'!$B$1,'کارنامه فردی'!$A$2:$A$26,0))</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -12782,7 +12761,7 @@
       </c>
       <c r="H7" s="7">
         <f>INDEX('کارنامه فردی'!AD2:AD26,MATCH('نتیجه فردی'!$B$1,'کارنامه فردی'!$A$2:$A$26,0))</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -12816,7 +12795,7 @@
       </c>
       <c r="H8" s="7">
         <f>INDEX('کارنامه فردی'!AM2:AM26,MATCH('نتیجه فردی'!$B$1,'کارنامه فردی'!$A$2:$A$26,0))</f>
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -12850,7 +12829,7 @@
       </c>
       <c r="H9" s="7">
         <f>INDEX('کارنامه فردی'!AV2:AV26,MATCH('نتیجه فردی'!$B$1,'کارنامه فردی'!$A$2:$A$26,0))</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -12884,7 +12863,7 @@
       </c>
       <c r="H10" s="7">
         <f>INDEX('کارنامه فردی'!BE2:BE26,MATCH('نتیجه فردی'!$B$1,'کارنامه فردی'!$A$2:$A$26,0))</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -12918,7 +12897,7 @@
       </c>
       <c r="H11" s="7">
         <f>INDEX('کارنامه فردی'!BN2:BN26,MATCH('نتیجه فردی'!$B$1,'کارنامه فردی'!$A$2:$A$26,0))</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -12952,7 +12931,7 @@
       </c>
       <c r="H12" s="7">
         <f>INDEX('کارنامه فردی'!BW2:BW26,MATCH('نتیجه فردی'!$B$1,'کارنامه فردی'!$A$2:$A$26,0))</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -13010,7 +12989,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13054,7 +13033,7 @@
       </c>
       <c r="J1" s="1" t="str">
         <f>_xlfn.CONCAT("  میانگین  ",D31,"  نفر برتر")</f>
-        <v xml:space="preserve">  میانگین  3  نفر برتر</v>
+        <v xml:space="preserve">  میانگین  10  نفر برتر</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -13096,7 +13075,7 @@
       </c>
       <c r="J2" s="6">
         <f>AVERAGEIF($A$2:$A$26,_xlfn.CONCAT("&lt;=",$D$31),$H$2:$H$26)</f>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -13138,7 +13117,7 @@
       </c>
       <c r="J3" s="6">
         <f t="shared" ref="J3:J26" si="3">AVERAGEIF($A$2:$A$26,_xlfn.CONCAT("&lt;=",$D$31),$H$2:$H$26)</f>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -13180,7 +13159,7 @@
       </c>
       <c r="J4" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -13222,7 +13201,7 @@
       </c>
       <c r="J5" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -13264,7 +13243,7 @@
       </c>
       <c r="J6" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -13306,7 +13285,7 @@
       </c>
       <c r="J7" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -13348,7 +13327,7 @@
       </c>
       <c r="J8" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -13390,7 +13369,7 @@
       </c>
       <c r="J9" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -13432,7 +13411,7 @@
       </c>
       <c r="J10" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -13474,7 +13453,7 @@
       </c>
       <c r="J11" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -13516,7 +13495,7 @@
       </c>
       <c r="J12" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -13558,7 +13537,7 @@
       </c>
       <c r="J13" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -13600,7 +13579,7 @@
       </c>
       <c r="J14" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -13642,7 +13621,7 @@
       </c>
       <c r="J15" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -13684,7 +13663,7 @@
       </c>
       <c r="J16" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -13726,7 +13705,7 @@
       </c>
       <c r="J17" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -13768,7 +13747,7 @@
       </c>
       <c r="J18" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -13810,7 +13789,7 @@
       </c>
       <c r="J19" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -13852,7 +13831,7 @@
       </c>
       <c r="J20" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -13894,7 +13873,7 @@
       </c>
       <c r="J21" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -13936,7 +13915,7 @@
       </c>
       <c r="J22" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -13978,7 +13957,7 @@
       </c>
       <c r="J23" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -14020,7 +13999,7 @@
       </c>
       <c r="J24" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -14062,7 +14041,7 @@
       </c>
       <c r="J25" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -14104,7 +14083,7 @@
       </c>
       <c r="J26" s="6">
         <f t="shared" si="3"/>
-        <v>73.333333333333329</v>
+        <v>14.242424242424242</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -14139,7 +14118,7 @@
       </c>
       <c r="D31" s="2">
         <f>تنظیمات!B7</f>
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -14176,7 +14155,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14237,1270 +14216,1270 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="45">
-        <f>ورودی!A2</f>
+      <c r="A2" s="44">
+        <f>'کارنامه فردی'!A2</f>
         <v>1001</v>
       </c>
-      <c r="B2" s="45" t="str">
-        <f>ورودی!B2</f>
+      <c r="B2" s="44" t="str">
+        <f>'کارنامه فردی'!B2</f>
         <v>a1</v>
       </c>
-      <c r="C2" s="45" t="str">
-        <f>ورودی!C2</f>
+      <c r="C2" s="44" t="str">
+        <f>'کارنامه فردی'!C2</f>
         <v>b1</v>
       </c>
-      <c r="D2" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="E2" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D2" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="E2" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="H2" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="H2" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I2" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I2" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J2" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>1</v>
-      </c>
-      <c r="K2" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L2" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J2" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L2" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="45">
-        <f>ورودی!A3</f>
+      <c r="A3" s="44">
+        <f>'کارنامه فردی'!A3</f>
         <v>1002</v>
       </c>
-      <c r="B3" s="45" t="str">
-        <f>ورودی!B3</f>
+      <c r="B3" s="44" t="str">
+        <f>'کارنامه فردی'!B3</f>
         <v>a2</v>
       </c>
-      <c r="C3" s="45" t="str">
-        <f>ورودی!C3</f>
+      <c r="C3" s="44" t="str">
+        <f>'کارنامه فردی'!C3</f>
         <v>b2</v>
       </c>
-      <c r="D3" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="F3" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D3" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>9</v>
+      </c>
+      <c r="G3" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>-3.33</v>
+      </c>
+      <c r="H3" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>100</v>
+      </c>
+      <c r="I3" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="H3" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>100</v>
-      </c>
-      <c r="I3" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>-33.33</v>
-      </c>
-      <c r="J3" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="J3" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>24</v>
       </c>
-      <c r="K3" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L3" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="K3" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L3" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="45">
-        <f>ورودی!A4</f>
+      <c r="A4" s="44">
+        <f>'کارنامه فردی'!A4</f>
         <v>1003</v>
       </c>
-      <c r="B4" s="45" t="str">
-        <f>ورودی!B4</f>
+      <c r="B4" s="44" t="str">
+        <f>'کارنامه فردی'!B4</f>
         <v>a3</v>
       </c>
-      <c r="C4" s="45" t="str">
-        <f>ورودی!C4</f>
+      <c r="C4" s="44" t="str">
+        <f>'کارنامه فردی'!C4</f>
         <v>b3</v>
       </c>
-      <c r="D4" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>3</v>
-      </c>
-      <c r="E4" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>2</v>
-      </c>
-      <c r="F4" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>46.67</v>
-      </c>
-      <c r="H4" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D4" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G4" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I4" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I4" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J4" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>3</v>
-      </c>
-      <c r="K4" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L4" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J4" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K4" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L4" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="45">
-        <f>ورودی!A5</f>
+      <c r="A5" s="44">
+        <f>'کارنامه فردی'!A5</f>
         <v>1004</v>
       </c>
-      <c r="B5" s="45" t="str">
-        <f>ورودی!B5</f>
+      <c r="B5" s="44" t="str">
+        <f>'کارنامه فردی'!B5</f>
         <v>a4</v>
       </c>
-      <c r="C5" s="45" t="str">
-        <f>ورودی!C5</f>
+      <c r="C5" s="44" t="str">
+        <f>'کارنامه فردی'!C5</f>
         <v>b4</v>
       </c>
-      <c r="D5" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G5" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D5" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G5" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I5" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I5" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J5" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K5" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L5" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J5" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K5" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L5" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="45">
-        <f>ورودی!A6</f>
+      <c r="A6" s="44">
+        <f>'کارنامه فردی'!A6</f>
         <v>1005</v>
       </c>
-      <c r="B6" s="45" t="str">
-        <f>ورودی!B6</f>
+      <c r="B6" s="44" t="str">
+        <f>'کارنامه فردی'!B6</f>
         <v>a5</v>
       </c>
-      <c r="C6" s="45" t="str">
-        <f>ورودی!C6</f>
+      <c r="C6" s="44" t="str">
+        <f>'کارنامه فردی'!C6</f>
         <v>b5</v>
       </c>
-      <c r="D6" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G6" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D6" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G6" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I6" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I6" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J6" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K6" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L6" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J6" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K6" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L6" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="45">
-        <f>ورودی!A7</f>
+      <c r="A7" s="44">
+        <f>'کارنامه فردی'!A7</f>
         <v>1006</v>
       </c>
-      <c r="B7" s="45" t="str">
-        <f>ورودی!B7</f>
+      <c r="B7" s="44" t="str">
+        <f>'کارنامه فردی'!B7</f>
         <v>a6</v>
       </c>
-      <c r="C7" s="45" t="str">
-        <f>ورودی!C7</f>
+      <c r="C7" s="44" t="str">
+        <f>'کارنامه فردی'!C7</f>
         <v>b6</v>
       </c>
-      <c r="D7" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G7" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D7" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G7" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I7" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I7" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J7" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K7" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L7" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J7" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K7" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L7" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="45">
-        <f>ورودی!A8</f>
+      <c r="A8" s="44">
+        <f>'کارنامه فردی'!A8</f>
         <v>1007</v>
       </c>
-      <c r="B8" s="45" t="str">
-        <f>ورودی!B8</f>
+      <c r="B8" s="44" t="str">
+        <f>'کارنامه فردی'!B8</f>
         <v>a7</v>
       </c>
-      <c r="C8" s="45" t="str">
-        <f>ورودی!C8</f>
+      <c r="C8" s="44" t="str">
+        <f>'کارنامه فردی'!C8</f>
         <v>b7</v>
       </c>
-      <c r="D8" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G8" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D8" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G8" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I8" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I8" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J8" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K8" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L8" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J8" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K8" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L8" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="45">
-        <f>ورودی!A9</f>
+      <c r="A9" s="44">
+        <f>'کارنامه فردی'!A9</f>
         <v>1008</v>
       </c>
-      <c r="B9" s="45" t="str">
-        <f>ورودی!B9</f>
+      <c r="B9" s="44" t="str">
+        <f>'کارنامه فردی'!B9</f>
         <v>a8</v>
       </c>
-      <c r="C9" s="45" t="str">
-        <f>ورودی!C9</f>
+      <c r="C9" s="44" t="str">
+        <f>'کارنامه فردی'!C9</f>
         <v>b8</v>
       </c>
-      <c r="D9" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D9" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G9" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="E9" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>5</v>
+      </c>
+      <c r="G9" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>50</v>
+      </c>
+      <c r="H9" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I9" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I9" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J9" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K9" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L9" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J9" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="K9" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L9" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="45">
-        <f>ورودی!A10</f>
+      <c r="A10" s="44">
+        <f>'کارنامه فردی'!A10</f>
         <v>1009</v>
       </c>
-      <c r="B10" s="45" t="str">
-        <f>ورودی!B10</f>
+      <c r="B10" s="44" t="str">
+        <f>'کارنامه فردی'!B10</f>
         <v>a9</v>
       </c>
-      <c r="C10" s="45" t="str">
-        <f>ورودی!C10</f>
+      <c r="C10" s="44" t="str">
+        <f>'کارنامه فردی'!C10</f>
         <v>b9</v>
       </c>
-      <c r="D10" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G10" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D10" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G10" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I10" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I10" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J10" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K10" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L10" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J10" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K10" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L10" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="45">
-        <f>ورودی!A11</f>
+      <c r="A11" s="44">
+        <f>'کارنامه فردی'!A11</f>
         <v>1010</v>
       </c>
-      <c r="B11" s="45" t="str">
-        <f>ورودی!B11</f>
+      <c r="B11" s="44" t="str">
+        <f>'کارنامه فردی'!B11</f>
         <v>a10</v>
       </c>
-      <c r="C11" s="45" t="str">
-        <f>ورودی!C11</f>
+      <c r="C11" s="44" t="str">
+        <f>'کارنامه فردی'!C11</f>
         <v>b10</v>
       </c>
-      <c r="D11" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G11" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D11" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G11" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I11" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I11" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J11" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K11" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L11" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J11" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K11" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L11" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="45">
-        <f>ورودی!A12</f>
+      <c r="A12" s="44">
+        <f>'کارنامه فردی'!A12</f>
         <v>1011</v>
       </c>
-      <c r="B12" s="45" t="str">
-        <f>ورودی!B12</f>
+      <c r="B12" s="44" t="str">
+        <f>'کارنامه فردی'!B12</f>
         <v>a11</v>
       </c>
-      <c r="C12" s="45" t="str">
-        <f>ورودی!C12</f>
+      <c r="C12" s="44" t="str">
+        <f>'کارنامه فردی'!C12</f>
         <v>b11</v>
       </c>
-      <c r="D12" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>3</v>
-      </c>
-      <c r="E12" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>2</v>
-      </c>
-      <c r="F12" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>46.67</v>
-      </c>
-      <c r="H12" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D12" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G12" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I12" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I12" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J12" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>3</v>
-      </c>
-      <c r="K12" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L12" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J12" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K12" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L12" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="45">
-        <f>ورودی!A13</f>
+      <c r="A13" s="44">
+        <f>'کارنامه فردی'!A13</f>
         <v>1012</v>
       </c>
-      <c r="B13" s="45" t="str">
-        <f>ورودی!B13</f>
+      <c r="B13" s="44" t="str">
+        <f>'کارنامه فردی'!B13</f>
         <v>a12</v>
       </c>
-      <c r="C13" s="45" t="str">
-        <f>ورودی!C13</f>
+      <c r="C13" s="44" t="str">
+        <f>'کارنامه فردی'!C13</f>
         <v>b12</v>
       </c>
-      <c r="D13" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>2</v>
-      </c>
-      <c r="E13" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>3</v>
-      </c>
-      <c r="F13" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>20</v>
-      </c>
-      <c r="H13" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D13" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G13" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I13" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I13" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J13" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="K13" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L13" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J13" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K13" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L13" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="45">
-        <f>ورودی!A14</f>
+      <c r="A14" s="44">
+        <f>'کارنامه فردی'!A14</f>
         <v>1013</v>
       </c>
-      <c r="B14" s="45" t="str">
-        <f>ورودی!B14</f>
+      <c r="B14" s="44" t="str">
+        <f>'کارنامه فردی'!B14</f>
         <v>a13</v>
       </c>
-      <c r="C14" s="45" t="str">
-        <f>ورودی!C14</f>
+      <c r="C14" s="44" t="str">
+        <f>'کارنامه فردی'!C14</f>
         <v>b13</v>
       </c>
-      <c r="D14" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G14" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D14" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G14" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I14" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I14" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J14" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K14" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L14" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J14" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K14" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L14" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="45">
-        <f>ورودی!A15</f>
+      <c r="A15" s="44">
+        <f>'کارنامه فردی'!A15</f>
         <v>1014</v>
       </c>
-      <c r="B15" s="45" t="str">
-        <f>ورودی!B15</f>
+      <c r="B15" s="44" t="str">
+        <f>'کارنامه فردی'!B15</f>
         <v>a14</v>
       </c>
-      <c r="C15" s="45" t="str">
-        <f>ورودی!C15</f>
+      <c r="C15" s="44" t="str">
+        <f>'کارنامه فردی'!C15</f>
         <v>b14</v>
       </c>
-      <c r="D15" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G15" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D15" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G15" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I15" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I15" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J15" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K15" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L15" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J15" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K15" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L15" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="45">
-        <f>ورودی!A16</f>
+      <c r="A16" s="44">
+        <f>'کارنامه فردی'!A16</f>
         <v>1015</v>
       </c>
-      <c r="B16" s="45" t="str">
-        <f>ورودی!B16</f>
+      <c r="B16" s="44" t="str">
+        <f>'کارنامه فردی'!B16</f>
         <v>a15</v>
       </c>
-      <c r="C16" s="45" t="str">
-        <f>ورودی!C16</f>
+      <c r="C16" s="44" t="str">
+        <f>'کارنامه فردی'!C16</f>
         <v>b15</v>
       </c>
-      <c r="D16" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G16" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D16" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G16" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I16" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I16" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J16" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K16" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L16" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J16" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K16" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L16" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="45">
-        <f>ورودی!A17</f>
+      <c r="A17" s="44">
+        <f>'کارنامه فردی'!A17</f>
         <v>1016</v>
       </c>
-      <c r="B17" s="45" t="str">
-        <f>ورودی!B17</f>
+      <c r="B17" s="44" t="str">
+        <f>'کارنامه فردی'!B17</f>
         <v>a16</v>
       </c>
-      <c r="C17" s="45" t="str">
-        <f>ورودی!C17</f>
+      <c r="C17" s="44" t="str">
+        <f>'کارنامه فردی'!C17</f>
         <v>b16</v>
       </c>
-      <c r="D17" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G17" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D17" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G17" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I17" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I17" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J17" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K17" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L17" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J17" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K17" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L17" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="45">
-        <f>ورودی!A18</f>
+      <c r="A18" s="44">
+        <f>'کارنامه فردی'!A18</f>
         <v>1017</v>
       </c>
-      <c r="B18" s="45" t="str">
-        <f>ورودی!B18</f>
+      <c r="B18" s="44" t="str">
+        <f>'کارنامه فردی'!B18</f>
         <v>a17</v>
       </c>
-      <c r="C18" s="45" t="str">
-        <f>ورودی!C18</f>
+      <c r="C18" s="44" t="str">
+        <f>'کارنامه فردی'!C18</f>
         <v>b17</v>
       </c>
-      <c r="D18" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G18" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D18" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G18" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I18" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I18" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J18" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K18" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L18" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J18" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K18" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L18" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="45">
-        <f>ورودی!A19</f>
+      <c r="A19" s="44">
+        <f>'کارنامه فردی'!A19</f>
         <v>1018</v>
       </c>
-      <c r="B19" s="45" t="str">
-        <f>ورودی!B19</f>
+      <c r="B19" s="44" t="str">
+        <f>'کارنامه فردی'!B19</f>
         <v>a18</v>
       </c>
-      <c r="C19" s="45" t="str">
-        <f>ورودی!C19</f>
+      <c r="C19" s="44" t="str">
+        <f>'کارنامه فردی'!C19</f>
         <v>b18</v>
       </c>
-      <c r="D19" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G19" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D19" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G19" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I19" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I19" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J19" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K19" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L19" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J19" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K19" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L19" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="45">
-        <f>ورودی!A20</f>
+      <c r="A20" s="44">
+        <f>'کارنامه فردی'!A20</f>
         <v>1019</v>
       </c>
-      <c r="B20" s="45" t="str">
-        <f>ورودی!B20</f>
+      <c r="B20" s="44" t="str">
+        <f>'کارنامه فردی'!B20</f>
         <v>a19</v>
       </c>
-      <c r="C20" s="45" t="str">
-        <f>ورودی!C20</f>
+      <c r="C20" s="44" t="str">
+        <f>'کارنامه فردی'!C20</f>
         <v>b19</v>
       </c>
-      <c r="D20" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G20" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D20" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G20" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I20" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I20" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J20" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K20" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L20" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J20" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K20" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L20" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="45">
-        <f>ورودی!A21</f>
+      <c r="A21" s="44">
+        <f>'کارنامه فردی'!A21</f>
         <v>1020</v>
       </c>
-      <c r="B21" s="45" t="str">
-        <f>ورودی!B21</f>
+      <c r="B21" s="44" t="str">
+        <f>'کارنامه فردی'!B21</f>
         <v>a20</v>
       </c>
-      <c r="C21" s="45" t="str">
-        <f>ورودی!C21</f>
+      <c r="C21" s="44" t="str">
+        <f>'کارنامه فردی'!C21</f>
         <v>b20</v>
       </c>
-      <c r="D21" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G21" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D21" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G21" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I21" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I21" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J21" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K21" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L21" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J21" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K21" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L21" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="45">
-        <f>ورودی!A22</f>
+      <c r="A22" s="44">
+        <f>'کارنامه فردی'!A22</f>
         <v>1021</v>
       </c>
-      <c r="B22" s="45" t="str">
-        <f>ورودی!B22</f>
+      <c r="B22" s="44" t="str">
+        <f>'کارنامه فردی'!B22</f>
         <v>a21</v>
       </c>
-      <c r="C22" s="45" t="str">
-        <f>ورودی!C22</f>
+      <c r="C22" s="44" t="str">
+        <f>'کارنامه فردی'!C22</f>
         <v>b21</v>
       </c>
-      <c r="D22" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G22" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D22" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G22" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I22" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I22" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J22" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K22" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L22" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J22" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K22" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L22" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="45">
-        <f>ورودی!A23</f>
+      <c r="A23" s="44">
+        <f>'کارنامه فردی'!A23</f>
         <v>1022</v>
       </c>
-      <c r="B23" s="45" t="str">
-        <f>ورودی!B23</f>
+      <c r="B23" s="44" t="str">
+        <f>'کارنامه فردی'!B23</f>
         <v>a22</v>
       </c>
-      <c r="C23" s="45" t="str">
-        <f>ورودی!C23</f>
+      <c r="C23" s="44" t="str">
+        <f>'کارنامه فردی'!C23</f>
         <v>b22</v>
       </c>
-      <c r="D23" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="G23" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D23" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G23" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I23" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I23" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J23" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>6</v>
-      </c>
-      <c r="K23" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L23" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J23" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="K23" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L23" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="45">
-        <f>ورودی!A24</f>
+      <c r="A24" s="44">
+        <f>'کارنامه فردی'!A24</f>
         <v>1023</v>
       </c>
-      <c r="B24" s="45" t="str">
-        <f>ورودی!B24</f>
+      <c r="B24" s="44" t="str">
+        <f>'کارنامه فردی'!B24</f>
         <v>a23</v>
       </c>
-      <c r="C24" s="45" t="str">
-        <f>ورودی!C24</f>
+      <c r="C24" s="44" t="str">
+        <f>'کارنامه فردی'!C24</f>
         <v>b23</v>
       </c>
-      <c r="D24" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F24" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D24" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="G24" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>100</v>
+      </c>
+      <c r="I24" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>-33.33</v>
+      </c>
+      <c r="J24" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>4</v>
       </c>
-      <c r="G24" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>-6.67</v>
-      </c>
-      <c r="H24" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>100</v>
-      </c>
-      <c r="I24" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>-33.33</v>
-      </c>
-      <c r="J24" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>23</v>
-      </c>
-      <c r="K24" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L24" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="K24" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L24" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="45">
-        <f>ورودی!A25</f>
+      <c r="A25" s="44">
+        <f>'کارنامه فردی'!A25</f>
         <v>1024</v>
       </c>
-      <c r="B25" s="45" t="str">
-        <f>ورودی!B25</f>
+      <c r="B25" s="44" t="str">
+        <f>'کارنامه فردی'!B25</f>
         <v>a24</v>
       </c>
-      <c r="C25" s="45" t="str">
-        <f>ورودی!C25</f>
+      <c r="C25" s="44" t="str">
+        <f>'کارنامه فردی'!C25</f>
         <v>b24</v>
       </c>
-      <c r="D25" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="F25" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D25" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="F25" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="H25" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="H25" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I25" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I25" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J25" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>24</v>
-      </c>
-      <c r="K25" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L25" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J25" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
+      </c>
+      <c r="K25" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L25" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="45">
-        <f>ورودی!A26</f>
+      <c r="A26" s="44">
+        <f>'کارنامه فردی'!A26</f>
         <v>1025</v>
       </c>
-      <c r="B26" s="45" t="str">
-        <f>ورودی!B26</f>
+      <c r="B26" s="44" t="str">
+        <f>'کارنامه فردی'!B26</f>
         <v>a25</v>
       </c>
-      <c r="C26" s="45" t="str">
-        <f>ورودی!C26</f>
+      <c r="C26" s="44" t="str">
+        <f>'کارنامه فردی'!C26</f>
         <v>b25</v>
       </c>
-      <c r="D26" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>5</v>
-      </c>
-      <c r="E26" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="D26" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>10</v>
+      </c>
+      <c r="E26" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="H26" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="H26" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I26" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+      <c r="I26" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J26" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>1</v>
-      </c>
-      <c r="K26" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>9.6</v>
-      </c>
-      <c r="L26" s="45">
-        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('نتیجه درسی جدید'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
-        <v>66.67</v>
+      <c r="J26" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="K26" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="L26" s="44">
+        <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="45" t="s">
-        <v>59</v>
+      <c r="C28" s="44" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="45">
+      <c r="C29" s="44">
         <f>تنظیمات!B7</f>
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -15537,7 +15516,7 @@
   <dimension ref="A1:GV30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="CA32" sqref="CA32"/>
+      <selection activeCell="BM31" sqref="BM31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16323,7 +16302,7 @@
       </c>
       <c r="L2" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M2" s="9">
         <f>COUNTIF(INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -16359,7 +16338,7 @@
       </c>
       <c r="U2" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V2" s="10">
         <f>COUNTIF(INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -16395,7 +16374,7 @@
       </c>
       <c r="AD2" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE2" s="11">
         <f>COUNTIF(INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -16431,7 +16410,7 @@
       </c>
       <c r="AM2" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN2" s="12">
         <f>COUNTIF(INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -16467,7 +16446,7 @@
       </c>
       <c r="AV2" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW2" s="24">
         <f>COUNTIF(INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -16503,7 +16482,7 @@
       </c>
       <c r="BE2" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF2" s="13">
         <f>COUNTIF(INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -16539,7 +16518,7 @@
       </c>
       <c r="BN2" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO2" s="14">
         <f>COUNTIF(INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D2:BK2,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -16575,7 +16554,7 @@
       </c>
       <c r="BW2" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX2" s="15">
         <f t="shared" ref="BX2:BX26" si="2">SUM(BO2,BF2,AN2,AE2,V2,M2,D2)</f>
@@ -17141,7 +17120,7 @@
       </c>
       <c r="L3" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M3" s="9">
         <f>COUNTIF(INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -17177,7 +17156,7 @@
       </c>
       <c r="U3" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V3" s="10">
         <f>COUNTIF(INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -17213,7 +17192,7 @@
       </c>
       <c r="AD3" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE3" s="11">
         <f>COUNTIF(INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -17249,7 +17228,7 @@
       </c>
       <c r="AM3" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN3" s="12">
         <f>COUNTIF(INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -17285,7 +17264,7 @@
       </c>
       <c r="AV3" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW3" s="24">
         <f>COUNTIF(INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -17321,7 +17300,7 @@
       </c>
       <c r="BE3" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF3" s="13">
         <f>COUNTIF(INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -17357,7 +17336,7 @@
       </c>
       <c r="BN3" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO3" s="14">
         <f>COUNTIF(INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D3:BK3,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -17393,7 +17372,7 @@
       </c>
       <c r="BW3" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX3" s="15">
         <f t="shared" si="2"/>
@@ -17959,7 +17938,7 @@
       </c>
       <c r="L4" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M4" s="9">
         <f>COUNTIF(INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -17995,7 +17974,7 @@
       </c>
       <c r="U4" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V4" s="10">
         <f>COUNTIF(INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -18031,7 +18010,7 @@
       </c>
       <c r="AD4" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE4" s="11">
         <f>COUNTIF(INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -18067,7 +18046,7 @@
       </c>
       <c r="AM4" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN4" s="12">
         <f>COUNTIF(INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -18103,7 +18082,7 @@
       </c>
       <c r="AV4" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW4" s="24">
         <f>COUNTIF(INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -18139,7 +18118,7 @@
       </c>
       <c r="BE4" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF4" s="13">
         <f>COUNTIF(INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -18175,7 +18154,7 @@
       </c>
       <c r="BN4" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO4" s="14">
         <f>COUNTIF(INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D4:BK4,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -18211,7 +18190,7 @@
       </c>
       <c r="BW4" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX4" s="15">
         <f t="shared" si="2"/>
@@ -18777,7 +18756,7 @@
       </c>
       <c r="L5" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M5" s="9">
         <f>COUNTIF(INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -18813,7 +18792,7 @@
       </c>
       <c r="U5" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V5" s="10">
         <f>COUNTIF(INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -18849,7 +18828,7 @@
       </c>
       <c r="AD5" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE5" s="11">
         <f>COUNTIF(INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -18885,7 +18864,7 @@
       </c>
       <c r="AM5" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN5" s="12">
         <f>COUNTIF(INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -18921,7 +18900,7 @@
       </c>
       <c r="AV5" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW5" s="24">
         <f>COUNTIF(INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -18957,7 +18936,7 @@
       </c>
       <c r="BE5" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF5" s="13">
         <f>COUNTIF(INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -18993,7 +18972,7 @@
       </c>
       <c r="BN5" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO5" s="14">
         <f>COUNTIF(INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D5:BK5,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -19029,7 +19008,7 @@
       </c>
       <c r="BW5" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX5" s="15">
         <f t="shared" si="2"/>
@@ -19595,7 +19574,7 @@
       </c>
       <c r="L6" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M6" s="9">
         <f>COUNTIF(INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -19631,7 +19610,7 @@
       </c>
       <c r="U6" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V6" s="10">
         <f>COUNTIF(INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -19667,7 +19646,7 @@
       </c>
       <c r="AD6" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE6" s="11">
         <f>COUNTIF(INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -19703,7 +19682,7 @@
       </c>
       <c r="AM6" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN6" s="12">
         <f>COUNTIF(INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -19739,7 +19718,7 @@
       </c>
       <c r="AV6" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW6" s="24">
         <f>COUNTIF(INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -19775,7 +19754,7 @@
       </c>
       <c r="BE6" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF6" s="13">
         <f>COUNTIF(INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -19811,7 +19790,7 @@
       </c>
       <c r="BN6" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO6" s="14">
         <f>COUNTIF(INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D6:BK6,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -19847,7 +19826,7 @@
       </c>
       <c r="BW6" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX6" s="15">
         <f t="shared" si="2"/>
@@ -20413,7 +20392,7 @@
       </c>
       <c r="L7" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M7" s="9">
         <f>COUNTIF(INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -20449,7 +20428,7 @@
       </c>
       <c r="U7" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V7" s="10">
         <f>COUNTIF(INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -20485,7 +20464,7 @@
       </c>
       <c r="AD7" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE7" s="11">
         <f>COUNTIF(INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -20521,7 +20500,7 @@
       </c>
       <c r="AM7" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN7" s="12">
         <f>COUNTIF(INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -20557,7 +20536,7 @@
       </c>
       <c r="AV7" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW7" s="24">
         <f>COUNTIF(INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -20593,7 +20572,7 @@
       </c>
       <c r="BE7" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF7" s="13">
         <f>COUNTIF(INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -20629,7 +20608,7 @@
       </c>
       <c r="BN7" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO7" s="14">
         <f>COUNTIF(INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D7:BK7,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -20665,7 +20644,7 @@
       </c>
       <c r="BW7" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX7" s="15">
         <f t="shared" si="2"/>
@@ -21231,7 +21210,7 @@
       </c>
       <c r="L8" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M8" s="9">
         <f>COUNTIF(INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -21267,7 +21246,7 @@
       </c>
       <c r="U8" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V8" s="10">
         <f>COUNTIF(INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -21303,7 +21282,7 @@
       </c>
       <c r="AD8" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE8" s="11">
         <f>COUNTIF(INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -21339,7 +21318,7 @@
       </c>
       <c r="AM8" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN8" s="12">
         <f>COUNTIF(INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -21375,7 +21354,7 @@
       </c>
       <c r="AV8" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW8" s="24">
         <f>COUNTIF(INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -21411,7 +21390,7 @@
       </c>
       <c r="BE8" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF8" s="13">
         <f>COUNTIF(INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -21447,7 +21426,7 @@
       </c>
       <c r="BN8" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO8" s="14">
         <f>COUNTIF(INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D8:BK8,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -21483,7 +21462,7 @@
       </c>
       <c r="BW8" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX8" s="15">
         <f t="shared" si="2"/>
@@ -22049,7 +22028,7 @@
       </c>
       <c r="L9" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M9" s="9">
         <f>COUNTIF(INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -22085,7 +22064,7 @@
       </c>
       <c r="U9" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V9" s="10">
         <f>COUNTIF(INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -22121,7 +22100,7 @@
       </c>
       <c r="AD9" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE9" s="11">
         <f>COUNTIF(INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -22157,7 +22136,7 @@
       </c>
       <c r="AM9" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN9" s="12">
         <f>COUNTIF(INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -22193,7 +22172,7 @@
       </c>
       <c r="AV9" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW9" s="24">
         <f>COUNTIF(INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -22229,7 +22208,7 @@
       </c>
       <c r="BE9" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF9" s="13">
         <f>COUNTIF(INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -22265,7 +22244,7 @@
       </c>
       <c r="BN9" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO9" s="14">
         <f>COUNTIF(INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D9:BK9,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -22301,7 +22280,7 @@
       </c>
       <c r="BW9" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX9" s="15">
         <f t="shared" si="2"/>
@@ -22867,7 +22846,7 @@
       </c>
       <c r="L10" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M10" s="9">
         <f>COUNTIF(INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -22903,7 +22882,7 @@
       </c>
       <c r="U10" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V10" s="10">
         <f>COUNTIF(INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -22939,7 +22918,7 @@
       </c>
       <c r="AD10" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE10" s="11">
         <f>COUNTIF(INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -22975,7 +22954,7 @@
       </c>
       <c r="AM10" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN10" s="12">
         <f>COUNTIF(INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -23011,7 +22990,7 @@
       </c>
       <c r="AV10" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW10" s="24">
         <f>COUNTIF(INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -23047,7 +23026,7 @@
       </c>
       <c r="BE10" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF10" s="13">
         <f>COUNTIF(INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -23083,7 +23062,7 @@
       </c>
       <c r="BN10" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO10" s="14">
         <f>COUNTIF(INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D10:BK10,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -23119,7 +23098,7 @@
       </c>
       <c r="BW10" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX10" s="15">
         <f t="shared" si="2"/>
@@ -23685,7 +23664,7 @@
       </c>
       <c r="L11" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M11" s="9">
         <f>COUNTIF(INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -23721,7 +23700,7 @@
       </c>
       <c r="U11" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V11" s="10">
         <f>COUNTIF(INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -23757,7 +23736,7 @@
       </c>
       <c r="AD11" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE11" s="11">
         <f>COUNTIF(INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -23793,7 +23772,7 @@
       </c>
       <c r="AM11" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN11" s="12">
         <f>COUNTIF(INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -23829,7 +23808,7 @@
       </c>
       <c r="AV11" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW11" s="24">
         <f>COUNTIF(INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -23865,7 +23844,7 @@
       </c>
       <c r="BE11" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF11" s="13">
         <f>COUNTIF(INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -23901,7 +23880,7 @@
       </c>
       <c r="BN11" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO11" s="14">
         <f>COUNTIF(INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D11:BK11,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -23937,7 +23916,7 @@
       </c>
       <c r="BW11" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX11" s="15">
         <f t="shared" si="2"/>
@@ -24503,7 +24482,7 @@
       </c>
       <c r="L12" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M12" s="9">
         <f>COUNTIF(INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -24539,7 +24518,7 @@
       </c>
       <c r="U12" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V12" s="10">
         <f>COUNTIF(INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -24575,7 +24554,7 @@
       </c>
       <c r="AD12" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE12" s="11">
         <f>COUNTIF(INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -24611,7 +24590,7 @@
       </c>
       <c r="AM12" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN12" s="12">
         <f>COUNTIF(INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -24647,7 +24626,7 @@
       </c>
       <c r="AV12" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW12" s="24">
         <f>COUNTIF(INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -24683,7 +24662,7 @@
       </c>
       <c r="BE12" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF12" s="13">
         <f>COUNTIF(INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -24719,7 +24698,7 @@
       </c>
       <c r="BN12" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO12" s="14">
         <f>COUNTIF(INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D12:BK12,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -24755,7 +24734,7 @@
       </c>
       <c r="BW12" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX12" s="15">
         <f t="shared" si="2"/>
@@ -25321,7 +25300,7 @@
       </c>
       <c r="L13" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M13" s="9">
         <f>COUNTIF(INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -25357,7 +25336,7 @@
       </c>
       <c r="U13" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V13" s="10">
         <f>COUNTIF(INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -25393,7 +25372,7 @@
       </c>
       <c r="AD13" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE13" s="11">
         <f>COUNTIF(INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -25429,7 +25408,7 @@
       </c>
       <c r="AM13" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN13" s="12">
         <f>COUNTIF(INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -25465,7 +25444,7 @@
       </c>
       <c r="AV13" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW13" s="24">
         <f>COUNTIF(INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -25501,7 +25480,7 @@
       </c>
       <c r="BE13" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF13" s="13">
         <f>COUNTIF(INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -25537,7 +25516,7 @@
       </c>
       <c r="BN13" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO13" s="14">
         <f>COUNTIF(INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D13:BK13,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -25573,7 +25552,7 @@
       </c>
       <c r="BW13" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX13" s="15">
         <f t="shared" si="2"/>
@@ -26139,7 +26118,7 @@
       </c>
       <c r="L14" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M14" s="9">
         <f>COUNTIF(INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -26175,7 +26154,7 @@
       </c>
       <c r="U14" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V14" s="10">
         <f>COUNTIF(INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -26211,7 +26190,7 @@
       </c>
       <c r="AD14" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE14" s="11">
         <f>COUNTIF(INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -26247,7 +26226,7 @@
       </c>
       <c r="AM14" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN14" s="12">
         <f>COUNTIF(INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -26283,7 +26262,7 @@
       </c>
       <c r="AV14" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW14" s="24">
         <f>COUNTIF(INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -26319,7 +26298,7 @@
       </c>
       <c r="BE14" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF14" s="13">
         <f>COUNTIF(INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -26355,7 +26334,7 @@
       </c>
       <c r="BN14" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO14" s="14">
         <f>COUNTIF(INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D14:BK14,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -26391,7 +26370,7 @@
       </c>
       <c r="BW14" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX14" s="15">
         <f t="shared" si="2"/>
@@ -26957,7 +26936,7 @@
       </c>
       <c r="L15" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M15" s="9">
         <f>COUNTIF(INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -26993,7 +26972,7 @@
       </c>
       <c r="U15" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V15" s="10">
         <f>COUNTIF(INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -27029,7 +27008,7 @@
       </c>
       <c r="AD15" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE15" s="11">
         <f>COUNTIF(INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -27065,7 +27044,7 @@
       </c>
       <c r="AM15" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN15" s="12">
         <f>COUNTIF(INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -27101,7 +27080,7 @@
       </c>
       <c r="AV15" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW15" s="24">
         <f>COUNTIF(INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -27137,7 +27116,7 @@
       </c>
       <c r="BE15" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF15" s="13">
         <f>COUNTIF(INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -27173,7 +27152,7 @@
       </c>
       <c r="BN15" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO15" s="14">
         <f>COUNTIF(INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D15:BK15,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -27209,7 +27188,7 @@
       </c>
       <c r="BW15" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX15" s="15">
         <f t="shared" si="2"/>
@@ -27775,7 +27754,7 @@
       </c>
       <c r="L16" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M16" s="9">
         <f>COUNTIF(INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -27811,7 +27790,7 @@
       </c>
       <c r="U16" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V16" s="10">
         <f>COUNTIF(INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -27847,7 +27826,7 @@
       </c>
       <c r="AD16" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE16" s="11">
         <f>COUNTIF(INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -27883,7 +27862,7 @@
       </c>
       <c r="AM16" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN16" s="12">
         <f>COUNTIF(INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -27919,7 +27898,7 @@
       </c>
       <c r="AV16" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW16" s="24">
         <f>COUNTIF(INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -27955,7 +27934,7 @@
       </c>
       <c r="BE16" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF16" s="13">
         <f>COUNTIF(INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -27991,7 +27970,7 @@
       </c>
       <c r="BN16" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO16" s="14">
         <f>COUNTIF(INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D16:BK16,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -28027,7 +28006,7 @@
       </c>
       <c r="BW16" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX16" s="15">
         <f t="shared" si="2"/>
@@ -28593,7 +28572,7 @@
       </c>
       <c r="L17" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M17" s="9">
         <f>COUNTIF(INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -28629,7 +28608,7 @@
       </c>
       <c r="U17" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V17" s="10">
         <f>COUNTIF(INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -28665,7 +28644,7 @@
       </c>
       <c r="AD17" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE17" s="11">
         <f>COUNTIF(INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -28701,7 +28680,7 @@
       </c>
       <c r="AM17" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN17" s="12">
         <f>COUNTIF(INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -28737,7 +28716,7 @@
       </c>
       <c r="AV17" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW17" s="24">
         <f>COUNTIF(INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -28773,7 +28752,7 @@
       </c>
       <c r="BE17" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF17" s="13">
         <f>COUNTIF(INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -28809,7 +28788,7 @@
       </c>
       <c r="BN17" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO17" s="14">
         <f>COUNTIF(INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D17:BK17,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -28845,7 +28824,7 @@
       </c>
       <c r="BW17" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX17" s="15">
         <f t="shared" si="2"/>
@@ -29411,7 +29390,7 @@
       </c>
       <c r="L18" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M18" s="9">
         <f>COUNTIF(INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -29447,7 +29426,7 @@
       </c>
       <c r="U18" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V18" s="10">
         <f>COUNTIF(INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -29483,7 +29462,7 @@
       </c>
       <c r="AD18" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE18" s="11">
         <f>COUNTIF(INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -29519,7 +29498,7 @@
       </c>
       <c r="AM18" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN18" s="12">
         <f>COUNTIF(INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -29555,7 +29534,7 @@
       </c>
       <c r="AV18" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW18" s="24">
         <f>COUNTIF(INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -29591,7 +29570,7 @@
       </c>
       <c r="BE18" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF18" s="13">
         <f>COUNTIF(INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -29627,7 +29606,7 @@
       </c>
       <c r="BN18" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO18" s="14">
         <f>COUNTIF(INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D18:BK18,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -29663,7 +29642,7 @@
       </c>
       <c r="BW18" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX18" s="15">
         <f t="shared" si="2"/>
@@ -30229,7 +30208,7 @@
       </c>
       <c r="L19" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M19" s="9">
         <f>COUNTIF(INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -30265,7 +30244,7 @@
       </c>
       <c r="U19" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V19" s="10">
         <f>COUNTIF(INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -30301,7 +30280,7 @@
       </c>
       <c r="AD19" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE19" s="11">
         <f>COUNTIF(INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -30337,7 +30316,7 @@
       </c>
       <c r="AM19" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN19" s="12">
         <f>COUNTIF(INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -30373,7 +30352,7 @@
       </c>
       <c r="AV19" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW19" s="24">
         <f>COUNTIF(INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -30409,7 +30388,7 @@
       </c>
       <c r="BE19" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF19" s="13">
         <f>COUNTIF(INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -30445,7 +30424,7 @@
       </c>
       <c r="BN19" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO19" s="14">
         <f>COUNTIF(INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D19:BK19,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -30481,7 +30460,7 @@
       </c>
       <c r="BW19" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX19" s="15">
         <f t="shared" si="2"/>
@@ -31047,7 +31026,7 @@
       </c>
       <c r="L20" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M20" s="9">
         <f>COUNTIF(INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -31083,7 +31062,7 @@
       </c>
       <c r="U20" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V20" s="10">
         <f>COUNTIF(INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -31119,7 +31098,7 @@
       </c>
       <c r="AD20" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE20" s="11">
         <f>COUNTIF(INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -31155,7 +31134,7 @@
       </c>
       <c r="AM20" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN20" s="12">
         <f>COUNTIF(INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -31191,7 +31170,7 @@
       </c>
       <c r="AV20" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW20" s="24">
         <f>COUNTIF(INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -31227,7 +31206,7 @@
       </c>
       <c r="BE20" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF20" s="13">
         <f>COUNTIF(INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -31263,7 +31242,7 @@
       </c>
       <c r="BN20" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO20" s="14">
         <f>COUNTIF(INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D20:BK20,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -31299,7 +31278,7 @@
       </c>
       <c r="BW20" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX20" s="15">
         <f t="shared" si="2"/>
@@ -31865,7 +31844,7 @@
       </c>
       <c r="L21" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M21" s="9">
         <f>COUNTIF(INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -31901,7 +31880,7 @@
       </c>
       <c r="U21" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V21" s="10">
         <f>COUNTIF(INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -31937,7 +31916,7 @@
       </c>
       <c r="AD21" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE21" s="11">
         <f>COUNTIF(INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -31973,7 +31952,7 @@
       </c>
       <c r="AM21" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN21" s="12">
         <f>COUNTIF(INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -32009,7 +31988,7 @@
       </c>
       <c r="AV21" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW21" s="24">
         <f>COUNTIF(INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -32045,7 +32024,7 @@
       </c>
       <c r="BE21" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF21" s="13">
         <f>COUNTIF(INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -32081,7 +32060,7 @@
       </c>
       <c r="BN21" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO21" s="14">
         <f>COUNTIF(INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D21:BK21,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -32117,7 +32096,7 @@
       </c>
       <c r="BW21" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX21" s="15">
         <f t="shared" si="2"/>
@@ -32683,7 +32662,7 @@
       </c>
       <c r="L22" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M22" s="9">
         <f>COUNTIF(INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -32719,7 +32698,7 @@
       </c>
       <c r="U22" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V22" s="10">
         <f>COUNTIF(INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -32755,7 +32734,7 @@
       </c>
       <c r="AD22" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE22" s="11">
         <f>COUNTIF(INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -32791,7 +32770,7 @@
       </c>
       <c r="AM22" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN22" s="12">
         <f>COUNTIF(INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -32827,7 +32806,7 @@
       </c>
       <c r="AV22" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW22" s="24">
         <f>COUNTIF(INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -32863,7 +32842,7 @@
       </c>
       <c r="BE22" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF22" s="13">
         <f>COUNTIF(INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -32899,7 +32878,7 @@
       </c>
       <c r="BN22" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO22" s="14">
         <f>COUNTIF(INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D22:BK22,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -32935,7 +32914,7 @@
       </c>
       <c r="BW22" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX22" s="15">
         <f t="shared" si="2"/>
@@ -33501,7 +33480,7 @@
       </c>
       <c r="L23" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M23" s="9">
         <f>COUNTIF(INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -33537,7 +33516,7 @@
       </c>
       <c r="U23" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V23" s="10">
         <f>COUNTIF(INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -33573,7 +33552,7 @@
       </c>
       <c r="AD23" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE23" s="11">
         <f>COUNTIF(INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -33609,7 +33588,7 @@
       </c>
       <c r="AM23" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN23" s="12">
         <f>COUNTIF(INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -33645,7 +33624,7 @@
       </c>
       <c r="AV23" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW23" s="24">
         <f>COUNTIF(INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -33681,7 +33660,7 @@
       </c>
       <c r="BE23" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF23" s="13">
         <f>COUNTIF(INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -33717,7 +33696,7 @@
       </c>
       <c r="BN23" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO23" s="14">
         <f>COUNTIF(INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D23:BK23,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -33753,7 +33732,7 @@
       </c>
       <c r="BW23" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX23" s="15">
         <f t="shared" si="2"/>
@@ -34319,7 +34298,7 @@
       </c>
       <c r="L24" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M24" s="9">
         <f>COUNTIF(INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -34355,7 +34334,7 @@
       </c>
       <c r="U24" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V24" s="10">
         <f>COUNTIF(INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -34391,7 +34370,7 @@
       </c>
       <c r="AD24" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE24" s="11">
         <f>COUNTIF(INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -34427,7 +34406,7 @@
       </c>
       <c r="AM24" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN24" s="12">
         <f>COUNTIF(INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -34463,7 +34442,7 @@
       </c>
       <c r="AV24" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW24" s="24">
         <f>COUNTIF(INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -34499,7 +34478,7 @@
       </c>
       <c r="BE24" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF24" s="13">
         <f>COUNTIF(INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -34535,7 +34514,7 @@
       </c>
       <c r="BN24" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO24" s="14">
         <f>COUNTIF(INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D24:BK24,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -34571,7 +34550,7 @@
       </c>
       <c r="BW24" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX24" s="15">
         <f t="shared" si="2"/>
@@ -35137,7 +35116,7 @@
       </c>
       <c r="L25" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M25" s="9">
         <f>COUNTIF(INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -35173,7 +35152,7 @@
       </c>
       <c r="U25" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V25" s="10">
         <f>COUNTIF(INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -35209,7 +35188,7 @@
       </c>
       <c r="AD25" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE25" s="11">
         <f>COUNTIF(INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -35245,7 +35224,7 @@
       </c>
       <c r="AM25" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN25" s="12">
         <f>COUNTIF(INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -35281,7 +35260,7 @@
       </c>
       <c r="AV25" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW25" s="24">
         <f>COUNTIF(INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -35317,7 +35296,7 @@
       </c>
       <c r="BE25" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF25" s="13">
         <f>COUNTIF(INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -35353,7 +35332,7 @@
       </c>
       <c r="BN25" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO25" s="14">
         <f>COUNTIF(INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D25:BK25,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -35389,7 +35368,7 @@
       </c>
       <c r="BW25" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX25" s="15">
         <f t="shared" si="2"/>
@@ -35955,7 +35934,7 @@
       </c>
       <c r="L26" s="38">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
-        <v>66.67</v>
+        <v>31.33</v>
       </c>
       <c r="M26" s="9">
         <f>COUNTIF(INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$C$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$C$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -35991,7 +35970,7 @@
       </c>
       <c r="U26" s="39">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="V26" s="10">
         <f>COUNTIF(INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$D$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$D$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -36027,7 +36006,7 @@
       </c>
       <c r="AD26" s="40">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AE26" s="11">
         <f>COUNTIF(INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$E$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$E$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -36063,7 +36042,7 @@
       </c>
       <c r="AM26" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AN26" s="12">
         <f>COUNTIF(INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$F$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$F$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -36099,7 +36078,7 @@
       </c>
       <c r="AV26" s="41">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
-        <v>66.67</v>
+        <v>25</v>
       </c>
       <c r="AW26" s="24">
         <f>COUNTIF(INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$G$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$G$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -36135,7 +36114,7 @@
       </c>
       <c r="BE26" s="24">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
-        <v>77.78</v>
+        <v>23.33</v>
       </c>
       <c r="BF26" s="13">
         <f>COUNTIF(INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$H$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$H$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -36171,7 +36150,7 @@
       </c>
       <c r="BN26" s="42">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
-        <v>83.33</v>
+        <v>25</v>
       </c>
       <c r="BO26" s="14">
         <f>COUNTIF(INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$I$3,خروجی!$D$1:$BK$1)):INDEX(خروجی!D26:BK26,MATCH(تنظیمات!$I$4,خروجی!$D$1:$BK$1)),3)</f>
@@ -36207,7 +36186,7 @@
       </c>
       <c r="BW26" s="43">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
-        <v>66.67</v>
+        <v>20</v>
       </c>
       <c r="BX26" s="15">
         <f t="shared" si="2"/>
@@ -36747,7 +36726,7 @@
   <dimension ref="A1:BI7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="BF13" sqref="BF13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37729,7 +37708,7 @@
   <dimension ref="A1:BK26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="BH17" sqref="BH17"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add min and max into reuslt docx
</commit_message>
<xml_diff>
--- a/quiz.xlsx
+++ b/quiz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Persons\Soroosh\Quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CAF8B1-451A-42A8-ADFB-FEAF26BA223C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F2C0A2-6367-4BFD-951E-7D38ED194038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -826,7 +826,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -923,22 +923,10 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4084,17 +4072,17 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -11563,1268 +11551,1268 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="40">
+      <c r="A2" s="36">
         <f>'کارنامه فردی'!A2</f>
         <v>1001</v>
       </c>
-      <c r="B2" s="40" t="str">
+      <c r="B2" s="36" t="str">
         <f>'کارنامه فردی'!B2</f>
         <v>a1</v>
       </c>
-      <c r="C2" s="40" t="str">
+      <c r="C2" s="36" t="str">
         <f>'کارنامه فردی'!C2</f>
         <v>b1</v>
       </c>
-      <c r="D2" s="40">
+      <c r="D2" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="E2" s="40">
+      <c r="E2" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F2" s="40">
+      <c r="F2" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="G2" s="40">
+      <c r="G2" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="H2" s="40">
+      <c r="H2" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I2" s="40">
+      <c r="I2" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J2" s="40">
+      <c r="J2" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>1</v>
       </c>
-      <c r="K2" s="40">
+      <c r="K2" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L2" s="40">
+      <c r="L2" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A2,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="40">
+      <c r="A3" s="36">
         <f>'کارنامه فردی'!A3</f>
         <v>1002</v>
       </c>
-      <c r="B3" s="40" t="str">
+      <c r="B3" s="36" t="str">
         <f>'کارنامه فردی'!B3</f>
         <v>a2</v>
       </c>
-      <c r="C3" s="40" t="str">
+      <c r="C3" s="36" t="str">
         <f>'کارنامه فردی'!C3</f>
         <v>b2</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G3" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="H3" s="40">
+      <c r="H3" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I3" s="40">
+      <c r="I3" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J3" s="40">
+      <c r="J3" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>24</v>
       </c>
-      <c r="K3" s="40">
+      <c r="K3" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L3" s="40">
+      <c r="L3" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A3,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="40">
+      <c r="A4" s="36">
         <f>'کارنامه فردی'!A4</f>
         <v>1003</v>
       </c>
-      <c r="B4" s="40" t="str">
+      <c r="B4" s="36" t="str">
         <f>'کارنامه فردی'!B4</f>
         <v>a3</v>
       </c>
-      <c r="C4" s="40" t="str">
+      <c r="C4" s="36" t="str">
         <f>'کارنامه فردی'!C4</f>
         <v>b3</v>
       </c>
-      <c r="D4" s="40">
+      <c r="D4" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>3</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>2</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="G4" s="40">
+      <c r="G4" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>46.67</v>
       </c>
-      <c r="H4" s="40">
+      <c r="H4" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I4" s="40">
+      <c r="I4" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J4" s="40">
+      <c r="J4" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>3</v>
       </c>
-      <c r="K4" s="40">
+      <c r="K4" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L4" s="40">
+      <c r="L4" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A4,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="40">
+      <c r="A5" s="36">
         <f>'کارنامه فردی'!A5</f>
         <v>1004</v>
       </c>
-      <c r="B5" s="40" t="str">
+      <c r="B5" s="36" t="str">
         <f>'کارنامه فردی'!B5</f>
         <v>a4</v>
       </c>
-      <c r="C5" s="40" t="str">
+      <c r="C5" s="36" t="str">
         <f>'کارنامه فردی'!C5</f>
         <v>b4</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F5" s="40">
+      <c r="F5" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G5" s="40">
+      <c r="G5" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H5" s="40">
+      <c r="H5" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I5" s="40">
+      <c r="I5" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J5" s="40">
+      <c r="J5" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K5" s="40">
+      <c r="K5" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L5" s="40">
+      <c r="L5" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A5,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="40">
+      <c r="A6" s="36">
         <f>'کارنامه فردی'!A6</f>
         <v>1005</v>
       </c>
-      <c r="B6" s="40" t="str">
+      <c r="B6" s="36" t="str">
         <f>'کارنامه فردی'!B6</f>
         <v>a5</v>
       </c>
-      <c r="C6" s="40" t="str">
+      <c r="C6" s="36" t="str">
         <f>'کارنامه فردی'!C6</f>
         <v>b5</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G6" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H6" s="40">
+      <c r="H6" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I6" s="40">
+      <c r="I6" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J6" s="40">
+      <c r="J6" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K6" s="40">
+      <c r="K6" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L6" s="40">
+      <c r="L6" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A6,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="40">
+      <c r="A7" s="36">
         <f>'کارنامه فردی'!A7</f>
         <v>1006</v>
       </c>
-      <c r="B7" s="40" t="str">
+      <c r="B7" s="36" t="str">
         <f>'کارنامه فردی'!B7</f>
         <v>a6</v>
       </c>
-      <c r="C7" s="40" t="str">
+      <c r="C7" s="36" t="str">
         <f>'کارنامه فردی'!C7</f>
         <v>b6</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H7" s="40">
+      <c r="H7" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I7" s="40">
+      <c r="I7" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J7" s="40">
+      <c r="J7" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K7" s="40">
+      <c r="K7" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L7" s="40">
+      <c r="L7" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A7,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="40">
+      <c r="A8" s="36">
         <f>'کارنامه فردی'!A8</f>
         <v>1007</v>
       </c>
-      <c r="B8" s="40" t="str">
+      <c r="B8" s="36" t="str">
         <f>'کارنامه فردی'!B8</f>
         <v>a7</v>
       </c>
-      <c r="C8" s="40" t="str">
+      <c r="C8" s="36" t="str">
         <f>'کارنامه فردی'!C8</f>
         <v>b7</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H8" s="40">
+      <c r="H8" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I8" s="40">
+      <c r="I8" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J8" s="40">
+      <c r="J8" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K8" s="40">
+      <c r="K8" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L8" s="40">
+      <c r="L8" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A8,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="40">
+      <c r="A9" s="36">
         <f>'کارنامه فردی'!A9</f>
         <v>1008</v>
       </c>
-      <c r="B9" s="40" t="str">
+      <c r="B9" s="36" t="str">
         <f>'کارنامه فردی'!B9</f>
         <v>a8</v>
       </c>
-      <c r="C9" s="40" t="str">
+      <c r="C9" s="36" t="str">
         <f>'کارنامه فردی'!C9</f>
         <v>b8</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H9" s="40">
+      <c r="H9" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I9" s="40">
+      <c r="I9" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J9" s="40">
+      <c r="J9" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K9" s="40">
+      <c r="K9" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L9" s="40">
+      <c r="L9" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A9,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="40">
+      <c r="A10" s="36">
         <f>'کارنامه فردی'!A10</f>
         <v>1009</v>
       </c>
-      <c r="B10" s="40" t="str">
+      <c r="B10" s="36" t="str">
         <f>'کارنامه فردی'!B10</f>
         <v>a9</v>
       </c>
-      <c r="C10" s="40" t="str">
+      <c r="C10" s="36" t="str">
         <f>'کارنامه فردی'!C10</f>
         <v>b9</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F10" s="40">
+      <c r="F10" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G10" s="40">
+      <c r="G10" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H10" s="40">
+      <c r="H10" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I10" s="40">
+      <c r="I10" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J10" s="40">
+      <c r="J10" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K10" s="40">
+      <c r="K10" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L10" s="40">
+      <c r="L10" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A10,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="40">
+      <c r="A11" s="36">
         <f>'کارنامه فردی'!A11</f>
         <v>1010</v>
       </c>
-      <c r="B11" s="40" t="str">
+      <c r="B11" s="36" t="str">
         <f>'کارنامه فردی'!B11</f>
         <v>a10</v>
       </c>
-      <c r="C11" s="40" t="str">
+      <c r="C11" s="36" t="str">
         <f>'کارنامه فردی'!C11</f>
         <v>b10</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G11" s="40">
+      <c r="G11" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H11" s="40">
+      <c r="H11" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I11" s="40">
+      <c r="I11" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J11" s="40">
+      <c r="J11" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K11" s="40">
+      <c r="K11" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L11" s="40">
+      <c r="L11" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A11,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="40">
+      <c r="A12" s="36">
         <f>'کارنامه فردی'!A12</f>
         <v>1011</v>
       </c>
-      <c r="B12" s="40" t="str">
+      <c r="B12" s="36" t="str">
         <f>'کارنامه فردی'!B12</f>
         <v>a11</v>
       </c>
-      <c r="C12" s="40" t="str">
+      <c r="C12" s="36" t="str">
         <f>'کارنامه فردی'!C12</f>
         <v>b11</v>
       </c>
-      <c r="D12" s="40">
+      <c r="D12" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>3</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>2</v>
       </c>
-      <c r="F12" s="40">
+      <c r="F12" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="G12" s="40">
+      <c r="G12" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>46.67</v>
       </c>
-      <c r="H12" s="40">
+      <c r="H12" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I12" s="40">
+      <c r="I12" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J12" s="40">
+      <c r="J12" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>3</v>
       </c>
-      <c r="K12" s="40">
+      <c r="K12" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L12" s="40">
+      <c r="L12" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A12,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="40">
+      <c r="A13" s="36">
         <f>'کارنامه فردی'!A13</f>
         <v>1012</v>
       </c>
-      <c r="B13" s="40" t="str">
+      <c r="B13" s="36" t="str">
         <f>'کارنامه فردی'!B13</f>
         <v>a12</v>
       </c>
-      <c r="C13" s="40" t="str">
+      <c r="C13" s="36" t="str">
         <f>'کارنامه فردی'!C13</f>
         <v>b12</v>
       </c>
-      <c r="D13" s="40">
+      <c r="D13" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>2</v>
       </c>
-      <c r="E13" s="40">
+      <c r="E13" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>3</v>
       </c>
-      <c r="F13" s="40">
+      <c r="F13" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>20</v>
       </c>
-      <c r="H13" s="40">
+      <c r="H13" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I13" s="40">
+      <c r="I13" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J13" s="40">
+      <c r="J13" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="K13" s="40">
+      <c r="K13" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L13" s="40">
+      <c r="L13" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A13,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="40">
+      <c r="A14" s="36">
         <f>'کارنامه فردی'!A14</f>
         <v>1013</v>
       </c>
-      <c r="B14" s="40" t="str">
+      <c r="B14" s="36" t="str">
         <f>'کارنامه فردی'!B14</f>
         <v>a13</v>
       </c>
-      <c r="C14" s="40" t="str">
+      <c r="C14" s="36" t="str">
         <f>'کارنامه فردی'!C14</f>
         <v>b13</v>
       </c>
-      <c r="D14" s="40">
+      <c r="D14" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E14" s="40">
+      <c r="E14" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F14" s="40">
+      <c r="F14" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G14" s="40">
+      <c r="G14" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H14" s="40">
+      <c r="H14" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I14" s="40">
+      <c r="I14" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J14" s="40">
+      <c r="J14" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K14" s="40">
+      <c r="K14" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L14" s="40">
+      <c r="L14" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A14,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="40">
+      <c r="A15" s="36">
         <f>'کارنامه فردی'!A15</f>
         <v>1014</v>
       </c>
-      <c r="B15" s="40" t="str">
+      <c r="B15" s="36" t="str">
         <f>'کارنامه فردی'!B15</f>
         <v>a14</v>
       </c>
-      <c r="C15" s="40" t="str">
+      <c r="C15" s="36" t="str">
         <f>'کارنامه فردی'!C15</f>
         <v>b14</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F15" s="40">
+      <c r="F15" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G15" s="40">
+      <c r="G15" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H15" s="40">
+      <c r="H15" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I15" s="40">
+      <c r="I15" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J15" s="40">
+      <c r="J15" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K15" s="40">
+      <c r="K15" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L15" s="40">
+      <c r="L15" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A15,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="40">
+      <c r="A16" s="36">
         <f>'کارنامه فردی'!A16</f>
         <v>1015</v>
       </c>
-      <c r="B16" s="40" t="str">
+      <c r="B16" s="36" t="str">
         <f>'کارنامه فردی'!B16</f>
         <v>a15</v>
       </c>
-      <c r="C16" s="40" t="str">
+      <c r="C16" s="36" t="str">
         <f>'کارنامه فردی'!C16</f>
         <v>b15</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E16" s="40">
+      <c r="E16" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F16" s="40">
+      <c r="F16" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G16" s="40">
+      <c r="G16" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H16" s="40">
+      <c r="H16" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I16" s="40">
+      <c r="I16" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J16" s="40">
+      <c r="J16" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K16" s="40">
+      <c r="K16" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L16" s="40">
+      <c r="L16" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A16,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="40">
+      <c r="A17" s="36">
         <f>'کارنامه فردی'!A17</f>
         <v>1016</v>
       </c>
-      <c r="B17" s="40" t="str">
+      <c r="B17" s="36" t="str">
         <f>'کارنامه فردی'!B17</f>
         <v>a16</v>
       </c>
-      <c r="C17" s="40" t="str">
+      <c r="C17" s="36" t="str">
         <f>'کارنامه فردی'!C17</f>
         <v>b16</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E17" s="40">
+      <c r="E17" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F17" s="40">
+      <c r="F17" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G17" s="40">
+      <c r="G17" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H17" s="40">
+      <c r="H17" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I17" s="40">
+      <c r="I17" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J17" s="40">
+      <c r="J17" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K17" s="40">
+      <c r="K17" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L17" s="40">
+      <c r="L17" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A17,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="40">
+      <c r="A18" s="36">
         <f>'کارنامه فردی'!A18</f>
         <v>1017</v>
       </c>
-      <c r="B18" s="40" t="str">
+      <c r="B18" s="36" t="str">
         <f>'کارنامه فردی'!B18</f>
         <v>a17</v>
       </c>
-      <c r="C18" s="40" t="str">
+      <c r="C18" s="36" t="str">
         <f>'کارنامه فردی'!C18</f>
         <v>b17</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E18" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F18" s="40">
+      <c r="F18" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G18" s="40">
+      <c r="G18" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H18" s="40">
+      <c r="H18" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I18" s="40">
+      <c r="I18" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J18" s="40">
+      <c r="J18" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K18" s="40">
+      <c r="K18" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L18" s="40">
+      <c r="L18" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A18,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="40">
+      <c r="A19" s="36">
         <f>'کارنامه فردی'!A19</f>
         <v>1018</v>
       </c>
-      <c r="B19" s="40" t="str">
+      <c r="B19" s="36" t="str">
         <f>'کارنامه فردی'!B19</f>
         <v>a18</v>
       </c>
-      <c r="C19" s="40" t="str">
+      <c r="C19" s="36" t="str">
         <f>'کارنامه فردی'!C19</f>
         <v>b18</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E19" s="40">
+      <c r="E19" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F19" s="40">
+      <c r="F19" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G19" s="40">
+      <c r="G19" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H19" s="40">
+      <c r="H19" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I19" s="40">
+      <c r="I19" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J19" s="40">
+      <c r="J19" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K19" s="40">
+      <c r="K19" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L19" s="40">
+      <c r="L19" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A19,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="40">
+      <c r="A20" s="36">
         <f>'کارنامه فردی'!A20</f>
         <v>1019</v>
       </c>
-      <c r="B20" s="40" t="str">
+      <c r="B20" s="36" t="str">
         <f>'کارنامه فردی'!B20</f>
         <v>a19</v>
       </c>
-      <c r="C20" s="40" t="str">
+      <c r="C20" s="36" t="str">
         <f>'کارنامه فردی'!C20</f>
         <v>b19</v>
       </c>
-      <c r="D20" s="40">
+      <c r="D20" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E20" s="40">
+      <c r="E20" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F20" s="40">
+      <c r="F20" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G20" s="40">
+      <c r="G20" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H20" s="40">
+      <c r="H20" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I20" s="40">
+      <c r="I20" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J20" s="40">
+      <c r="J20" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K20" s="40">
+      <c r="K20" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L20" s="40">
+      <c r="L20" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A20,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="40">
+      <c r="A21" s="36">
         <f>'کارنامه فردی'!A21</f>
         <v>1020</v>
       </c>
-      <c r="B21" s="40" t="str">
+      <c r="B21" s="36" t="str">
         <f>'کارنامه فردی'!B21</f>
         <v>a20</v>
       </c>
-      <c r="C21" s="40" t="str">
+      <c r="C21" s="36" t="str">
         <f>'کارنامه فردی'!C21</f>
         <v>b20</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E21" s="40">
+      <c r="E21" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F21" s="40">
+      <c r="F21" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G21" s="40">
+      <c r="G21" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H21" s="40">
+      <c r="H21" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I21" s="40">
+      <c r="I21" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J21" s="40">
+      <c r="J21" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K21" s="40">
+      <c r="K21" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L21" s="40">
+      <c r="L21" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A21,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="40">
+      <c r="A22" s="36">
         <f>'کارنامه فردی'!A22</f>
         <v>1021</v>
       </c>
-      <c r="B22" s="40" t="str">
+      <c r="B22" s="36" t="str">
         <f>'کارنامه فردی'!B22</f>
         <v>a21</v>
       </c>
-      <c r="C22" s="40" t="str">
+      <c r="C22" s="36" t="str">
         <f>'کارنامه فردی'!C22</f>
         <v>b21</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F22" s="40">
+      <c r="F22" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G22" s="40">
+      <c r="G22" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H22" s="40">
+      <c r="H22" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I22" s="40">
+      <c r="I22" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J22" s="40">
+      <c r="J22" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K22" s="40">
+      <c r="K22" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L22" s="40">
+      <c r="L22" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A22,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="40">
+      <c r="A23" s="36">
         <f>'کارنامه فردی'!A23</f>
         <v>1022</v>
       </c>
-      <c r="B23" s="40" t="str">
+      <c r="B23" s="36" t="str">
         <f>'کارنامه فردی'!B23</f>
         <v>a22</v>
       </c>
-      <c r="C23" s="40" t="str">
+      <c r="C23" s="36" t="str">
         <f>'کارنامه فردی'!C23</f>
         <v>b22</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E23" s="40">
+      <c r="E23" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F23" s="40">
+      <c r="F23" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="G23" s="40">
+      <c r="G23" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="H23" s="40">
+      <c r="H23" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I23" s="40">
+      <c r="I23" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J23" s="40">
+      <c r="J23" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>6</v>
       </c>
-      <c r="K23" s="40">
+      <c r="K23" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L23" s="40">
+      <c r="L23" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A23,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="40">
+      <c r="A24" s="36">
         <f>'کارنامه فردی'!A24</f>
         <v>1023</v>
       </c>
-      <c r="B24" s="40" t="str">
+      <c r="B24" s="36" t="str">
         <f>'کارنامه فردی'!B24</f>
         <v>a23</v>
       </c>
-      <c r="C24" s="40" t="str">
+      <c r="C24" s="36" t="str">
         <f>'کارنامه فردی'!C24</f>
         <v>b23</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E24" s="40">
+      <c r="E24" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>1</v>
       </c>
-      <c r="F24" s="40">
+      <c r="F24" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>4</v>
       </c>
-      <c r="G24" s="40">
+      <c r="G24" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-6.67</v>
       </c>
-      <c r="H24" s="40">
+      <c r="H24" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I24" s="40">
+      <c r="I24" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J24" s="40">
+      <c r="J24" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>23</v>
       </c>
-      <c r="K24" s="40">
+      <c r="K24" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L24" s="40">
+      <c r="L24" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A24,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="40">
+      <c r="A25" s="36">
         <f>'کارنامه فردی'!A25</f>
         <v>1024</v>
       </c>
-      <c r="B25" s="40" t="str">
+      <c r="B25" s="36" t="str">
         <f>'کارنامه فردی'!B25</f>
         <v>a24</v>
       </c>
-      <c r="C25" s="40" t="str">
+      <c r="C25" s="36" t="str">
         <f>'کارنامه فردی'!C25</f>
         <v>b24</v>
       </c>
-      <c r="D25" s="40">
+      <c r="D25" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="E25" s="40">
+      <c r="E25" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="F25" s="40">
+      <c r="F25" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="G25" s="40">
+      <c r="G25" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="H25" s="40">
+      <c r="H25" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I25" s="40">
+      <c r="I25" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J25" s="40">
+      <c r="J25" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>24</v>
       </c>
-      <c r="K25" s="40">
+      <c r="K25" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L25" s="40">
+      <c r="L25" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A25,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="40">
+      <c r="A26" s="36">
         <f>'کارنامه فردی'!A26</f>
         <v>1025</v>
       </c>
-      <c r="B26" s="40" t="str">
+      <c r="B26" s="36" t="str">
         <f>'کارنامه فردی'!B26</f>
         <v>a25</v>
       </c>
-      <c r="C26" s="40" t="str">
+      <c r="C26" s="36" t="str">
         <f>'کارنامه فردی'!C26</f>
         <v>b25</v>
       </c>
-      <c r="D26" s="40">
+      <c r="D26" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(D$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>5</v>
       </c>
-      <c r="E26" s="40">
+      <c r="E26" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(E$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="F26" s="40">
+      <c r="F26" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(F$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>0</v>
       </c>
-      <c r="G26" s="40">
+      <c r="G26" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(G$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="H26" s="40">
+      <c r="H26" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(H$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>100</v>
       </c>
-      <c r="I26" s="40">
+      <c r="I26" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(I$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>-33.33</v>
       </c>
-      <c r="J26" s="40">
+      <c r="J26" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(J$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>1</v>
       </c>
-      <c r="K26" s="40">
+      <c r="K26" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(K$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>9.6</v>
       </c>
-      <c r="L26" s="40">
+      <c r="L26" s="36">
         <f>INDEX('کارنامه فردی'!$D$2:$BW$26,MATCH('کارنامه فردی'!$A26,'کارنامه فردی'!$A$2:$A$26,0),MATCH(_xlfn.CONCAT(L$1," ",$C$28),'کارنامه فردی'!$D$1:$BW$1,0))</f>
         <v>31.33</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="36" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="40">
+      <c r="C29" s="36">
         <f>تنظیمات!B7</f>
         <v>10</v>
       </c>
@@ -13845,7 +13833,7 @@
   <dimension ref="A1:GV30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14629,7 +14617,7 @@
         <f>ROUND(AVERAGE($G$2:$G$26),2)</f>
         <v>9.6</v>
       </c>
-      <c r="L2" s="34">
+      <c r="L2" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -14665,7 +14653,7 @@
         <f>ROUND(AVERAGE($P$2:$P$26),2)</f>
         <v>12</v>
       </c>
-      <c r="U2" s="35">
+      <c r="U2" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -14701,7 +14689,7 @@
         <f>ROUND(AVERAGE($Y$2:$Y$26),2)</f>
         <v>12</v>
       </c>
-      <c r="AD2" s="36">
+      <c r="AD2" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -14737,7 +14725,7 @@
         <f>ROUND(AVERAGE($AH$2:$AH$26),2)</f>
         <v>12</v>
       </c>
-      <c r="AM2" s="20">
+      <c r="AM2" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -14773,7 +14761,7 @@
         <f>ROUND(AVERAGE($AQ$2:$AQ$26),2)</f>
         <v>8.67</v>
       </c>
-      <c r="AV2" s="37">
+      <c r="AV2" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -14809,7 +14797,7 @@
         <f>ROUND(AVERAGE($AZ$2:$AZ$26),2)</f>
         <v>8</v>
       </c>
-      <c r="BE2" s="20">
+      <c r="BE2" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -14845,7 +14833,7 @@
         <f>ROUND(AVERAGE($BI$2:$BI$26),2)</f>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN2" s="38">
+      <c r="BN2" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -14881,7 +14869,7 @@
         <f>ROUND( AVERAGE($BR$2:$BR$26),2)</f>
         <v>6.67</v>
       </c>
-      <c r="BW2" s="39">
+      <c r="BW2" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -15447,7 +15435,7 @@
         <f t="shared" ref="K3:K26" si="8">ROUND(AVERAGE($G$2:$G$26),2)</f>
         <v>9.6</v>
       </c>
-      <c r="L3" s="34">
+      <c r="L3" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -15483,7 +15471,7 @@
         <f t="shared" ref="T3:T26" si="11">ROUND(AVERAGE($P$2:$P$26),2)</f>
         <v>12</v>
       </c>
-      <c r="U3" s="35">
+      <c r="U3" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -15519,7 +15507,7 @@
         <f t="shared" ref="AC3:AC26" si="16">ROUND(AVERAGE($Y$2:$Y$26),2)</f>
         <v>12</v>
       </c>
-      <c r="AD3" s="36">
+      <c r="AD3" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -15555,7 +15543,7 @@
         <f t="shared" ref="AL3:AL26" si="21">ROUND(AVERAGE($AH$2:$AH$26),2)</f>
         <v>12</v>
       </c>
-      <c r="AM3" s="20">
+      <c r="AM3" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -15591,7 +15579,7 @@
         <f t="shared" ref="AU3:AU26" si="26">ROUND(AVERAGE($AQ$2:$AQ$26),2)</f>
         <v>8.67</v>
       </c>
-      <c r="AV3" s="37">
+      <c r="AV3" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -15627,7 +15615,7 @@
         <f t="shared" ref="BD3:BD26" si="31">ROUND(AVERAGE($AZ$2:$AZ$26),2)</f>
         <v>8</v>
       </c>
-      <c r="BE3" s="20">
+      <c r="BE3" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -15663,7 +15651,7 @@
         <f t="shared" ref="BM3:BM26" si="36">ROUND(AVERAGE($BI$2:$BI$26),2)</f>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN3" s="38">
+      <c r="BN3" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -15699,7 +15687,7 @@
         <f t="shared" ref="BV3:BV26" si="41">ROUND( AVERAGE($BR$2:$BR$26),2)</f>
         <v>6.67</v>
       </c>
-      <c r="BW3" s="39">
+      <c r="BW3" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -16265,7 +16253,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L4" s="34">
+      <c r="L4" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -16301,7 +16289,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U4" s="35">
+      <c r="U4" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -16337,7 +16325,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD4" s="36">
+      <c r="AD4" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -16373,7 +16361,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM4" s="20">
+      <c r="AM4" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -16409,7 +16397,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV4" s="37">
+      <c r="AV4" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -16445,7 +16433,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE4" s="20">
+      <c r="BE4" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -16481,7 +16469,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN4" s="38">
+      <c r="BN4" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -16517,7 +16505,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW4" s="39">
+      <c r="BW4" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -17083,7 +17071,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L5" s="34">
+      <c r="L5" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -17119,7 +17107,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U5" s="35">
+      <c r="U5" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -17155,7 +17143,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD5" s="36">
+      <c r="AD5" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -17191,7 +17179,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM5" s="20">
+      <c r="AM5" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -17227,7 +17215,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV5" s="37">
+      <c r="AV5" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -17263,7 +17251,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE5" s="20">
+      <c r="BE5" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -17299,7 +17287,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN5" s="38">
+      <c r="BN5" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -17335,7 +17323,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW5" s="39">
+      <c r="BW5" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -17901,7 +17889,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L6" s="34">
+      <c r="L6" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -17937,7 +17925,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U6" s="35">
+      <c r="U6" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -17973,7 +17961,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD6" s="36">
+      <c r="AD6" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -18009,7 +17997,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM6" s="20">
+      <c r="AM6" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -18045,7 +18033,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV6" s="37">
+      <c r="AV6" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -18081,7 +18069,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE6" s="20">
+      <c r="BE6" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -18117,7 +18105,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN6" s="38">
+      <c r="BN6" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -18153,7 +18141,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW6" s="39">
+      <c r="BW6" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -18719,7 +18707,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L7" s="34">
+      <c r="L7" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -18755,7 +18743,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U7" s="35">
+      <c r="U7" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -18791,7 +18779,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD7" s="36">
+      <c r="AD7" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -18827,7 +18815,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM7" s="20">
+      <c r="AM7" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -18863,7 +18851,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV7" s="37">
+      <c r="AV7" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -18899,7 +18887,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE7" s="20">
+      <c r="BE7" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -18935,7 +18923,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN7" s="38">
+      <c r="BN7" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -18971,7 +18959,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW7" s="39">
+      <c r="BW7" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -19537,7 +19525,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L8" s="34">
+      <c r="L8" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -19573,7 +19561,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U8" s="35">
+      <c r="U8" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -19609,7 +19597,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD8" s="36">
+      <c r="AD8" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -19645,7 +19633,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM8" s="20">
+      <c r="AM8" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -19681,7 +19669,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV8" s="37">
+      <c r="AV8" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -19717,7 +19705,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE8" s="20">
+      <c r="BE8" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -19753,7 +19741,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN8" s="38">
+      <c r="BN8" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -19789,7 +19777,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW8" s="39">
+      <c r="BW8" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -20355,7 +20343,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L9" s="34">
+      <c r="L9" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -20391,7 +20379,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U9" s="35">
+      <c r="U9" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -20427,7 +20415,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD9" s="36">
+      <c r="AD9" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -20463,7 +20451,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM9" s="20">
+      <c r="AM9" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -20499,7 +20487,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV9" s="37">
+      <c r="AV9" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -20535,7 +20523,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE9" s="20">
+      <c r="BE9" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -20571,7 +20559,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN9" s="38">
+      <c r="BN9" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -20607,7 +20595,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW9" s="39">
+      <c r="BW9" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -21173,7 +21161,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L10" s="34">
+      <c r="L10" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -21209,7 +21197,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U10" s="35">
+      <c r="U10" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -21245,7 +21233,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD10" s="36">
+      <c r="AD10" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -21281,7 +21269,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM10" s="20">
+      <c r="AM10" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -21317,7 +21305,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV10" s="37">
+      <c r="AV10" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -21353,7 +21341,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE10" s="20">
+      <c r="BE10" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -21389,7 +21377,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN10" s="38">
+      <c r="BN10" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -21425,7 +21413,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW10" s="39">
+      <c r="BW10" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -21991,7 +21979,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L11" s="34">
+      <c r="L11" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -22027,7 +22015,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U11" s="35">
+      <c r="U11" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -22063,7 +22051,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD11" s="36">
+      <c r="AD11" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -22099,7 +22087,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM11" s="20">
+      <c r="AM11" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -22135,7 +22123,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV11" s="37">
+      <c r="AV11" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -22171,7 +22159,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE11" s="20">
+      <c r="BE11" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -22207,7 +22195,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN11" s="38">
+      <c r="BN11" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -22243,7 +22231,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW11" s="39">
+      <c r="BW11" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -22809,7 +22797,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L12" s="34">
+      <c r="L12" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -22845,7 +22833,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U12" s="35">
+      <c r="U12" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -22881,7 +22869,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD12" s="36">
+      <c r="AD12" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -22917,7 +22905,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM12" s="20">
+      <c r="AM12" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -22953,7 +22941,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV12" s="37">
+      <c r="AV12" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -22989,7 +22977,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE12" s="20">
+      <c r="BE12" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -23025,7 +23013,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN12" s="38">
+      <c r="BN12" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -23061,7 +23049,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW12" s="39">
+      <c r="BW12" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -23627,7 +23615,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L13" s="34">
+      <c r="L13" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -23663,7 +23651,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U13" s="35">
+      <c r="U13" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -23699,7 +23687,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD13" s="36">
+      <c r="AD13" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -23735,7 +23723,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM13" s="20">
+      <c r="AM13" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -23771,7 +23759,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV13" s="37">
+      <c r="AV13" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -23807,7 +23795,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE13" s="20">
+      <c r="BE13" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -23843,7 +23831,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN13" s="38">
+      <c r="BN13" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -23879,7 +23867,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW13" s="39">
+      <c r="BW13" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -24445,7 +24433,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L14" s="34">
+      <c r="L14" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -24481,7 +24469,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U14" s="35">
+      <c r="U14" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -24517,7 +24505,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD14" s="36">
+      <c r="AD14" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -24553,7 +24541,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM14" s="20">
+      <c r="AM14" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -24589,7 +24577,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV14" s="37">
+      <c r="AV14" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -24625,7 +24613,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE14" s="20">
+      <c r="BE14" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -24661,7 +24649,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN14" s="38">
+      <c r="BN14" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -24697,7 +24685,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW14" s="39">
+      <c r="BW14" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -25263,7 +25251,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L15" s="34">
+      <c r="L15" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -25299,7 +25287,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U15" s="35">
+      <c r="U15" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -25335,7 +25323,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD15" s="36">
+      <c r="AD15" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -25371,7 +25359,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM15" s="20">
+      <c r="AM15" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -25407,7 +25395,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV15" s="37">
+      <c r="AV15" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -25443,7 +25431,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE15" s="20">
+      <c r="BE15" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -25479,7 +25467,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN15" s="38">
+      <c r="BN15" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -25515,7 +25503,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW15" s="39">
+      <c r="BW15" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -26081,7 +26069,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L16" s="34">
+      <c r="L16" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -26117,7 +26105,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U16" s="35">
+      <c r="U16" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -26153,7 +26141,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD16" s="36">
+      <c r="AD16" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -26189,7 +26177,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM16" s="20">
+      <c r="AM16" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -26225,7 +26213,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV16" s="37">
+      <c r="AV16" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -26261,7 +26249,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE16" s="20">
+      <c r="BE16" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -26297,7 +26285,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN16" s="38">
+      <c r="BN16" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -26333,7 +26321,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW16" s="39">
+      <c r="BW16" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -26899,7 +26887,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L17" s="34">
+      <c r="L17" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -26935,7 +26923,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U17" s="35">
+      <c r="U17" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -26971,7 +26959,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD17" s="36">
+      <c r="AD17" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -27007,7 +26995,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM17" s="20">
+      <c r="AM17" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -27043,7 +27031,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV17" s="37">
+      <c r="AV17" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -27079,7 +27067,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE17" s="20">
+      <c r="BE17" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -27115,7 +27103,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN17" s="38">
+      <c r="BN17" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -27151,7 +27139,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW17" s="39">
+      <c r="BW17" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -27717,7 +27705,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L18" s="34">
+      <c r="L18" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -27753,7 +27741,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U18" s="35">
+      <c r="U18" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -27789,7 +27777,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD18" s="36">
+      <c r="AD18" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -27825,7 +27813,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM18" s="20">
+      <c r="AM18" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -27861,7 +27849,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV18" s="37">
+      <c r="AV18" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -27897,7 +27885,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE18" s="20">
+      <c r="BE18" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -27933,7 +27921,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN18" s="38">
+      <c r="BN18" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -27969,7 +27957,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW18" s="39">
+      <c r="BW18" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -28535,7 +28523,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L19" s="34">
+      <c r="L19" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -28571,7 +28559,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U19" s="35">
+      <c r="U19" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -28607,7 +28595,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD19" s="36">
+      <c r="AD19" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -28643,7 +28631,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM19" s="20">
+      <c r="AM19" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -28679,7 +28667,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV19" s="37">
+      <c r="AV19" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -28715,7 +28703,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE19" s="20">
+      <c r="BE19" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -28751,7 +28739,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN19" s="38">
+      <c r="BN19" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -28787,7 +28775,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW19" s="39">
+      <c r="BW19" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -29353,7 +29341,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L20" s="34">
+      <c r="L20" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -29389,7 +29377,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U20" s="35">
+      <c r="U20" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -29425,7 +29413,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD20" s="36">
+      <c r="AD20" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -29461,7 +29449,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM20" s="20">
+      <c r="AM20" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -29497,7 +29485,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV20" s="37">
+      <c r="AV20" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -29533,7 +29521,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE20" s="20">
+      <c r="BE20" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -29569,7 +29557,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN20" s="38">
+      <c r="BN20" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -29605,7 +29593,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW20" s="39">
+      <c r="BW20" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -30171,7 +30159,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L21" s="34">
+      <c r="L21" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -30207,7 +30195,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U21" s="35">
+      <c r="U21" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -30243,7 +30231,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD21" s="36">
+      <c r="AD21" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -30279,7 +30267,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM21" s="20">
+      <c r="AM21" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -30315,7 +30303,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV21" s="37">
+      <c r="AV21" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -30351,7 +30339,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE21" s="20">
+      <c r="BE21" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -30387,7 +30375,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN21" s="38">
+      <c r="BN21" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -30423,7 +30411,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW21" s="39">
+      <c r="BW21" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -30989,7 +30977,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L22" s="34">
+      <c r="L22" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -31025,7 +31013,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U22" s="35">
+      <c r="U22" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -31061,7 +31049,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD22" s="36">
+      <c r="AD22" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -31097,7 +31085,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM22" s="20">
+      <c r="AM22" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -31133,7 +31121,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV22" s="37">
+      <c r="AV22" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -31169,7 +31157,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE22" s="20">
+      <c r="BE22" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -31205,7 +31193,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN22" s="38">
+      <c r="BN22" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -31241,7 +31229,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW22" s="39">
+      <c r="BW22" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -31807,7 +31795,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L23" s="34">
+      <c r="L23" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -31843,7 +31831,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U23" s="35">
+      <c r="U23" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -31879,7 +31867,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD23" s="36">
+      <c r="AD23" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -31915,7 +31903,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM23" s="20">
+      <c r="AM23" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -31951,7 +31939,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV23" s="37">
+      <c r="AV23" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -31987,7 +31975,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE23" s="20">
+      <c r="BE23" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -32023,7 +32011,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN23" s="38">
+      <c r="BN23" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -32059,7 +32047,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW23" s="39">
+      <c r="BW23" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -32625,7 +32613,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L24" s="34">
+      <c r="L24" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -32661,7 +32649,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U24" s="35">
+      <c r="U24" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -32697,7 +32685,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD24" s="36">
+      <c r="AD24" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -32733,7 +32721,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM24" s="20">
+      <c r="AM24" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -32769,7 +32757,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV24" s="37">
+      <c r="AV24" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -32805,7 +32793,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE24" s="20">
+      <c r="BE24" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -32841,7 +32829,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN24" s="38">
+      <c r="BN24" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -32877,7 +32865,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW24" s="39">
+      <c r="BW24" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -33443,7 +33431,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L25" s="34">
+      <c r="L25" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -33479,7 +33467,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U25" s="35">
+      <c r="U25" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -33515,7 +33503,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD25" s="36">
+      <c r="AD25" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -33551,7 +33539,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM25" s="20">
+      <c r="AM25" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -33587,7 +33575,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV25" s="37">
+      <c r="AV25" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -33623,7 +33611,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE25" s="20">
+      <c r="BE25" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -33659,7 +33647,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN25" s="38">
+      <c r="BN25" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -33695,7 +33683,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW25" s="39">
+      <c r="BW25" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>
@@ -34261,7 +34249,7 @@
         <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
-      <c r="L26" s="34">
+      <c r="L26" s="23">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$G$2:$G$26),2)</f>
         <v>31.33</v>
       </c>
@@ -34297,7 +34285,7 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="U26" s="35">
+      <c r="U26" s="34">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$P$2:$P$26),2)</f>
         <v>40</v>
       </c>
@@ -34333,7 +34321,7 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="AD26" s="36">
+      <c r="AD26" s="25">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$Y$2:$Y$26),2)</f>
         <v>40</v>
       </c>
@@ -34369,7 +34357,7 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="AM26" s="20">
+      <c r="AM26" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AH$2:$AH$26),2)</f>
         <v>40</v>
       </c>
@@ -34405,7 +34393,7 @@
         <f t="shared" si="26"/>
         <v>8.67</v>
       </c>
-      <c r="AV26" s="37">
+      <c r="AV26" s="27">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AQ$2:$AQ$26),2)</f>
         <v>25</v>
       </c>
@@ -34441,7 +34429,7 @@
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="BE26" s="20">
+      <c r="BE26" s="26">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$AZ$2:$AZ$26),2)</f>
         <v>23.33</v>
       </c>
@@ -34477,7 +34465,7 @@
         <f t="shared" si="36"/>
         <v>8.5299999999999994</v>
       </c>
-      <c r="BN26" s="38">
+      <c r="BN26" s="35">
         <f>ROUND(AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BI$2:$BI$26),2)</f>
         <v>25</v>
       </c>
@@ -34513,7 +34501,7 @@
         <f t="shared" si="41"/>
         <v>6.67</v>
       </c>
-      <c r="BW26" s="39">
+      <c r="BW26" s="29">
         <f>ROUND( AVERAGEIF($CD$2:$CD$26,_xlfn.CONCAT("&lt;=",تنظیمات!$B$7),$BR$2:$BR$26),2)</f>
         <v>20</v>
       </c>

</xml_diff>